<commit_message>
defini secciones al website. prepare pruebas unitarias para paginas y ControladorDeCatalogo.
</commit_message>
<xml_diff>
--- a/dev_docs/scrum products.xlsx
+++ b/dev_docs/scrum products.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="panorama" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>======================</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Historias de usuario</t>
   </si>
   <si>
-    <t>Quiero aprender el vocabulario coloquial y el tecnico (los escenarios apropiados para el contexto)</t>
-  </si>
-  <si>
     <t>prioridad</t>
   </si>
   <si>
-    <t>numero de historias:</t>
-  </si>
-  <si>
     <t>Quiero que se tomen en cuenta los dispositivos moviles</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>Quiero que la arquitectura considere trabajar con varias bases de datos.</t>
   </si>
   <si>
-    <t>Quiero que soporte módulos instalables desde la misma.</t>
-  </si>
-  <si>
     <t>ZULUG - Scrum Web Tool</t>
   </si>
   <si>
@@ -167,13 +158,301 @@
   </si>
   <si>
     <t>Quiero que sea una comuniddad que pueda beneficiarse con las características de planktom y pueda contribuir en algun proceso de desarrollo.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">quiero un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>controlador</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con las tareas comunes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> los </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>catálogos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (listar, crear, guardar, eliminar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">de ser necesario quiero un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>objeto javascript</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que se comunique </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>con</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>controlador de catalogo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quiero que soporte </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>módulos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>instalables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> desde la misma.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">quiero que el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">modelo del catalogo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pueda comunicarse con modelos de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PDO, doctrine, Propel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>quiero que el nucleo tenga un api, generada con los comentarios en el codigo fuente</t>
+  </si>
+  <si>
+    <t>quiero un manual paso a paso con proyectos de ejemplo</t>
+  </si>
+  <si>
+    <t>crear un modulo para administrar y editar las paginas con html y estilos</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">crear un modulo para editar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>plantillas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>twig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en un editor html</t>
+    </r>
+  </si>
+  <si>
+    <t>Quiero que use efectos parallax</t>
+  </si>
+  <si>
+    <t>workload</t>
+  </si>
+  <si>
+    <t>No H</t>
+  </si>
+  <si>
+    <t>Quiero aprender el vocabulario coloquial y el tecnico considerando el contexto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +470,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -238,16 +525,10 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -265,6 +546,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -274,9 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -285,8 +569,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,422 +873,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="63.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="80.28515625" customWidth="1"/>
+    <col min="4" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="K1">
-        <f>SUM(K4:K26)</f>
+      <c r="D2" s="12"/>
+      <c r="J2">
+        <f>SUM(J5:J27)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>SUM(A4:A15)</f>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SUM(A5:A16)</f>
         <v>78</v>
       </c>
-      <c r="B2">
-        <f>SUM(B4:B15)</f>
+      <c r="B3">
+        <f>SUM(B5:B16)</f>
         <v>78</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="11"/>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>14</v>
-      </c>
-      <c r="F2" s="16" t="s">
+      <c r="J4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>6.5</v>
+      </c>
+      <c r="O5">
+        <f>N5*5*2</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4">
-        <v>16</v>
-      </c>
-      <c r="O4">
-        <v>6.5</v>
-      </c>
-      <c r="P4">
-        <f>O4*5*2</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
+      <c r="B7">
         <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="I7">
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="I8">
+      <c r="D9" s="12"/>
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="H10">
         <v>6</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="I9">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="H11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="H13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="H14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="H15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="I10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11">
-        <v>16</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="I12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="I13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>11</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="I14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
+  <mergeCells count="31">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,49 +1277,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM(A4:A11)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="6"/>
       <c r="H2" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4">
@@ -1069,13 +1330,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C6" s="12"/>
     </row>
@@ -1084,23 +1345,66 @@
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1109,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,63 +1425,73 @@
     <col min="3" max="3" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I1">
-        <f>SUM(I4:I22)</f>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>SUM(I6:I23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>SUM(A4:A11)</f>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SUM(A6:A12)</f>
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="H2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="19" t="s">
+      <c r="E3" s="6"/>
+      <c r="H3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1206,38 +1520,38 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="6"/>
       <c r="H2" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1580,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1276,62 +1590,62 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1355,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>